<commit_message>
v2.0: Implementación de equivalencias - Reducción 53.4%
</commit_message>
<xml_diff>
--- a/datos/Malla_Curricular_LLYA.xlsx
+++ b/datos/Malla_Curricular_LLYA.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="588" uniqueCount="90">
   <si>
     <t>PROGRAMA</t>
   </si>
@@ -79,9 +79,6 @@
   </si>
   <si>
     <t>Aula</t>
-  </si>
-  <si>
-    <t>Laboratorio</t>
   </si>
   <si>
     <t>Tarde</t>
@@ -563,7 +560,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="20.13"/>
     <col customWidth="1" min="2" max="2" width="23.13"/>
-    <col customWidth="1" min="3" max="3" width="36.13"/>
+    <col customWidth="1" min="3" max="3" width="27.5"/>
     <col customWidth="1" min="4" max="4" width="15.88"/>
     <col customWidth="1" min="7" max="8" width="18.0"/>
     <col customWidth="1" min="10" max="10" width="18.25"/>
@@ -662,10 +659,10 @@
         <v>21</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="3">
@@ -676,7 +673,7 @@
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4">
         <v>2778.0</v>
@@ -710,10 +707,10 @@
         <v>21</v>
       </c>
       <c r="N3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O3" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O3" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="4">
@@ -724,7 +721,7 @@
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" s="4">
         <v>5109.0</v>
@@ -758,10 +755,10 @@
         <v>21</v>
       </c>
       <c r="N4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O4" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="5">
@@ -772,7 +769,7 @@
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="4">
         <v>1366.0</v>
@@ -806,7 +803,7 @@
         <v>21</v>
       </c>
       <c r="O5" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6">
@@ -817,7 +814,7 @@
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="4">
         <v>9166.0</v>
@@ -851,7 +848,7 @@
         <v>21</v>
       </c>
       <c r="O6" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7">
@@ -862,7 +859,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="4">
         <v>1033.0</v>
@@ -877,7 +874,7 @@
         <v>2.0</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I7" s="5" t="s">
         <v>20</v>
@@ -893,10 +890,10 @@
         <v>4</v>
       </c>
       <c r="N7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8">
@@ -907,7 +904,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4">
         <v>5881.0</v>
@@ -941,7 +938,7 @@
         <v>21</v>
       </c>
       <c r="O8" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9">
@@ -952,7 +949,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D9" s="4">
         <v>2533.0</v>
@@ -986,10 +983,10 @@
         <v>21</v>
       </c>
       <c r="N9" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O9" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O9" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10">
@@ -1000,7 +997,7 @@
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D10" s="4">
         <v>9584.0</v>
@@ -1018,7 +1015,7 @@
         <v>19</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J10" s="5">
         <v>1.0</v>
@@ -1031,13 +1028,13 @@
         <v>3</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O10" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11">
@@ -1048,7 +1045,7 @@
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D11" s="4">
         <v>6701.0</v>
@@ -1063,7 +1060,7 @@
         <v>4.0</v>
       </c>
       <c r="H11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>20</v>
@@ -1082,10 +1079,10 @@
         <v>21</v>
       </c>
       <c r="N11" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O11" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="12">
@@ -1096,7 +1093,7 @@
         <v>16</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D12" s="4">
         <v>5476.0</v>
@@ -1111,7 +1108,7 @@
         <v>3.0</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>20</v>
@@ -1130,10 +1127,10 @@
         <v>21</v>
       </c>
       <c r="N12" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O12" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="13">
@@ -1144,7 +1141,7 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D13" s="4">
         <v>7720.0</v>
@@ -1162,7 +1159,7 @@
         <v>19</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J13" s="5">
         <v>4.0</v>
@@ -1175,13 +1172,13 @@
         <v>4</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N13" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14">
@@ -1192,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="4">
         <v>7187.0</v>
@@ -1207,7 +1204,7 @@
         <v>3.0</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>20</v>
@@ -1226,7 +1223,7 @@
         <v>21</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15">
@@ -1237,7 +1234,7 @@
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D15" s="4">
         <v>1909.0</v>
@@ -1252,7 +1249,7 @@
         <v>4.0</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>20</v>
@@ -1271,10 +1268,10 @@
         <v>21</v>
       </c>
       <c r="N15" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O15" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O15" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="16">
@@ -1285,7 +1282,7 @@
         <v>16</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D16" s="4">
         <v>2003.0</v>
@@ -1300,10 +1297,10 @@
         <v>4.0</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J16" s="5">
         <v>3.0</v>
@@ -1316,13 +1313,13 @@
         <v>5</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17">
@@ -1333,7 +1330,7 @@
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4">
         <v>9842.0</v>
@@ -1348,7 +1345,7 @@
         <v>4.0</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I17" s="5" t="s">
         <v>20</v>
@@ -1367,10 +1364,10 @@
         <v>21</v>
       </c>
       <c r="N17" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O17" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O17" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="18">
@@ -1381,7 +1378,7 @@
         <v>16</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D18" s="4">
         <v>5431.0</v>
@@ -1396,7 +1393,7 @@
         <v>3.0</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I18" s="5" t="s">
         <v>20</v>
@@ -1415,10 +1412,10 @@
         <v>21</v>
       </c>
       <c r="N18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O18" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O18" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="19">
@@ -1429,7 +1426,7 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D19" s="4">
         <v>5448.0</v>
@@ -1463,10 +1460,10 @@
         <v>21</v>
       </c>
       <c r="N19" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O19" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O19" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="20">
@@ -1477,7 +1474,7 @@
         <v>16</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D20" s="4">
         <v>4490.0</v>
@@ -1495,7 +1492,7 @@
         <v>19</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J20" s="5">
         <v>2.0</v>
@@ -1508,13 +1505,13 @@
         <v>4</v>
       </c>
       <c r="M20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N20" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O20" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21">
@@ -1525,7 +1522,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D21" s="4">
         <v>8330.0</v>
@@ -1543,7 +1540,7 @@
         <v>19</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J21" s="5">
         <v>3.0</v>
@@ -1556,13 +1553,13 @@
         <v>3</v>
       </c>
       <c r="M21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N21" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O21" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="22">
@@ -1573,7 +1570,7 @@
         <v>16</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D22" s="4">
         <v>3252.0</v>
@@ -1588,7 +1585,7 @@
         <v>2.0</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I22" s="5" t="s">
         <v>20</v>
@@ -1604,10 +1601,10 @@
         <v>4</v>
       </c>
       <c r="N22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O22" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23">
@@ -1618,7 +1615,7 @@
         <v>16</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D23" s="4">
         <v>4432.0</v>
@@ -1633,10 +1630,10 @@
         <v>4.0</v>
       </c>
       <c r="H23" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J23" s="5">
         <v>3.0</v>
@@ -1649,13 +1646,13 @@
         <v>5</v>
       </c>
       <c r="M23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O23" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24">
@@ -1666,7 +1663,7 @@
         <v>16</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="4">
         <v>4661.0</v>
@@ -1681,7 +1678,7 @@
         <v>4.0</v>
       </c>
       <c r="H24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I24" s="5" t="s">
         <v>20</v>
@@ -1700,10 +1697,10 @@
         <v>21</v>
       </c>
       <c r="N24" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O24" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O24" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="25">
@@ -1714,7 +1711,7 @@
         <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="4">
         <v>3064.0</v>
@@ -1748,10 +1745,10 @@
         <v>21</v>
       </c>
       <c r="N25" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O25" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O25" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="26">
@@ -1762,7 +1759,7 @@
         <v>16</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D26" s="4">
         <v>2434.0</v>
@@ -1796,7 +1793,7 @@
         <v>21</v>
       </c>
       <c r="O26" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27">
@@ -1807,7 +1804,7 @@
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D27" s="4">
         <v>8726.0</v>
@@ -1822,7 +1819,7 @@
         <v>3.0</v>
       </c>
       <c r="H27" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I27" s="5" t="s">
         <v>20</v>
@@ -1841,10 +1838,10 @@
         <v>21</v>
       </c>
       <c r="N27" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O27" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O27" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="28">
@@ -1855,7 +1852,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D28" s="4">
         <v>8518.0</v>
@@ -1889,10 +1886,10 @@
         <v>21</v>
       </c>
       <c r="N28" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O28" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O28" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="29">
@@ -1903,7 +1900,7 @@
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D29" s="4">
         <v>8717.0</v>
@@ -1918,7 +1915,7 @@
         <v>4.0</v>
       </c>
       <c r="H29" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I29" s="5" t="s">
         <v>20</v>
@@ -1937,10 +1934,10 @@
         <v>21</v>
       </c>
       <c r="N29" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O29" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O29" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="30">
@@ -1951,7 +1948,7 @@
         <v>16</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D30" s="4">
         <v>4604.0</v>
@@ -1985,10 +1982,10 @@
         <v>21</v>
       </c>
       <c r="N30" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O30" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O30" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="31">
@@ -1999,7 +1996,7 @@
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D31" s="4">
         <v>8588.0</v>
@@ -2033,7 +2030,7 @@
         <v>21</v>
       </c>
       <c r="O31" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32">
@@ -2044,7 +2041,7 @@
         <v>16</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D32" s="4">
         <v>3079.0</v>
@@ -2062,7 +2059,7 @@
         <v>19</v>
       </c>
       <c r="I32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J32" s="5">
         <v>1.0</v>
@@ -2075,13 +2072,13 @@
         <v>5</v>
       </c>
       <c r="M32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N32" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O32" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="33">
@@ -2092,7 +2089,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D33" s="4">
         <v>1512.0</v>
@@ -2126,10 +2123,10 @@
         <v>21</v>
       </c>
       <c r="N33" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O33" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O33" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="34">
@@ -2140,7 +2137,7 @@
         <v>16</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D34" s="4">
         <v>1793.0</v>
@@ -2174,10 +2171,10 @@
         <v>21</v>
       </c>
       <c r="N34" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O34" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="35">
@@ -2188,7 +2185,7 @@
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D35" s="4">
         <v>4202.0</v>
@@ -2222,10 +2219,10 @@
         <v>21</v>
       </c>
       <c r="N35" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O35" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="36">
@@ -2236,7 +2233,7 @@
         <v>16</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="4">
         <v>2063.0</v>
@@ -2251,7 +2248,7 @@
         <v>4.0</v>
       </c>
       <c r="H36" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I36" s="5" t="s">
         <v>20</v>
@@ -2270,10 +2267,10 @@
         <v>21</v>
       </c>
       <c r="N36" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O36" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O36" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="37">
@@ -2284,7 +2281,7 @@
         <v>16</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D37" s="4">
         <v>5423.0</v>
@@ -2302,7 +2299,7 @@
         <v>19</v>
       </c>
       <c r="I37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J37" s="5">
         <v>3.0</v>
@@ -2315,13 +2312,13 @@
         <v>3</v>
       </c>
       <c r="M37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O37" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="38">
@@ -2332,7 +2329,7 @@
         <v>16</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D38" s="4">
         <v>7045.0</v>
@@ -2347,7 +2344,7 @@
         <v>3.0</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I38" s="5" t="s">
         <v>20</v>
@@ -2366,7 +2363,7 @@
         <v>21</v>
       </c>
       <c r="O38" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="39">
@@ -2377,7 +2374,7 @@
         <v>16</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D39" s="4">
         <v>4629.0</v>
@@ -2392,7 +2389,7 @@
         <v>3.0</v>
       </c>
       <c r="H39" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I39" s="5" t="s">
         <v>20</v>
@@ -2411,10 +2408,10 @@
         <v>21</v>
       </c>
       <c r="N39" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O39" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O39" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="40">
@@ -2425,7 +2422,7 @@
         <v>16</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D40" s="4">
         <v>7113.0</v>
@@ -2440,7 +2437,7 @@
         <v>3.0</v>
       </c>
       <c r="H40" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I40" s="5" t="s">
         <v>20</v>
@@ -2459,10 +2456,10 @@
         <v>21</v>
       </c>
       <c r="N40" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O40" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O40" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="41">
@@ -2473,7 +2470,7 @@
         <v>16</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D41" s="4">
         <v>8636.0</v>
@@ -2488,7 +2485,7 @@
         <v>3.0</v>
       </c>
       <c r="H41" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>20</v>
@@ -2507,10 +2504,10 @@
         <v>21</v>
       </c>
       <c r="N41" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O41" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O41" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="42">
@@ -2521,7 +2518,7 @@
         <v>16</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D42" s="4">
         <v>6776.0</v>
@@ -2555,10 +2552,10 @@
         <v>21</v>
       </c>
       <c r="N42" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O42" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O42" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="43">
@@ -2569,7 +2566,7 @@
         <v>16</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43" s="4">
         <v>7627.0</v>
@@ -2584,7 +2581,7 @@
         <v>4.0</v>
       </c>
       <c r="H43" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I43" s="5" t="s">
         <v>20</v>
@@ -2603,10 +2600,10 @@
         <v>21</v>
       </c>
       <c r="N43" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O43" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O43" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="44">
@@ -2617,7 +2614,7 @@
         <v>16</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D44" s="4">
         <v>1822.0</v>
@@ -2651,10 +2648,10 @@
         <v>21</v>
       </c>
       <c r="N44" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O44" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O44" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="45">
@@ -2665,7 +2662,7 @@
         <v>16</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D45" s="4">
         <v>7794.0</v>
@@ -2699,7 +2696,7 @@
         <v>21</v>
       </c>
       <c r="O45" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="46">
@@ -2710,7 +2707,7 @@
         <v>16</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D46" s="4">
         <v>9734.0</v>
@@ -2725,7 +2722,7 @@
         <v>3.0</v>
       </c>
       <c r="H46" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I46" s="5" t="s">
         <v>20</v>
@@ -2744,10 +2741,10 @@
         <v>21</v>
       </c>
       <c r="N46" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O46" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O46" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="47">
@@ -2758,7 +2755,7 @@
         <v>16</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D47" s="4">
         <v>5080.0</v>
@@ -2773,7 +2770,7 @@
         <v>3.0</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I47" s="5" t="s">
         <v>20</v>
@@ -2792,10 +2789,10 @@
         <v>21</v>
       </c>
       <c r="N47" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O47" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O47" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="48">
@@ -2806,7 +2803,7 @@
         <v>16</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D48" s="4">
         <v>3762.0</v>
@@ -2840,10 +2837,10 @@
         <v>21</v>
       </c>
       <c r="N48" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O48" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O48" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="49">
@@ -2854,7 +2851,7 @@
         <v>16</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D49" s="4">
         <v>9807.0</v>
@@ -2888,10 +2885,10 @@
         <v>21</v>
       </c>
       <c r="N49" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O49" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O49" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="50">
@@ -2902,7 +2899,7 @@
         <v>16</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D50" s="4">
         <v>7773.0</v>
@@ -2936,7 +2933,7 @@
         <v>21</v>
       </c>
       <c r="O50" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="51">
@@ -2947,7 +2944,7 @@
         <v>16</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D51" s="4">
         <v>1240.0</v>
@@ -2981,10 +2978,10 @@
         <v>21</v>
       </c>
       <c r="N51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O51" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O51" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="52">
@@ -2995,7 +2992,7 @@
         <v>16</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D52" s="4">
         <v>2632.0</v>
@@ -3013,7 +3010,7 @@
         <v>19</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J52" s="5">
         <v>2.0</v>
@@ -3026,13 +3023,13 @@
         <v>4</v>
       </c>
       <c r="M52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N52" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O52" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="53">
@@ -3043,7 +3040,7 @@
         <v>16</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D53" s="4">
         <v>6434.0</v>
@@ -3058,7 +3055,7 @@
         <v>3.0</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I53" s="5" t="s">
         <v>20</v>
@@ -3077,10 +3074,10 @@
         <v>21</v>
       </c>
       <c r="N53" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O53" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O53" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="54">
@@ -3091,7 +3088,7 @@
         <v>16</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D54" s="4">
         <v>1804.0</v>
@@ -3106,7 +3103,7 @@
         <v>2.0</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I54" s="5" t="s">
         <v>20</v>
@@ -3122,10 +3119,10 @@
         <v>4</v>
       </c>
       <c r="N54" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O54" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="55">
@@ -3136,7 +3133,7 @@
         <v>16</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D55" s="4">
         <v>9935.0</v>
@@ -3151,7 +3148,7 @@
         <v>3.0</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I55" s="5" t="s">
         <v>20</v>
@@ -3170,10 +3167,10 @@
         <v>21</v>
       </c>
       <c r="N55" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O55" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O55" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="56">
@@ -3184,13 +3181,13 @@
         <v>16</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D56" s="4">
         <v>5166.0</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F56" s="5">
         <v>8.0</v>
@@ -3202,7 +3199,7 @@
         <v>19</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J56" s="5">
         <v>1.0</v>
@@ -3215,13 +3212,13 @@
         <v>3</v>
       </c>
       <c r="M56" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N56" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57">
@@ -3232,7 +3229,7 @@
         <v>16</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D57" s="4">
         <v>6050.0</v>
@@ -3247,7 +3244,7 @@
         <v>4.0</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I57" s="5" t="s">
         <v>20</v>
@@ -3266,10 +3263,10 @@
         <v>21</v>
       </c>
       <c r="N57" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O57" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O57" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="58">
@@ -3280,7 +3277,7 @@
         <v>16</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D58" s="4">
         <v>5079.0</v>
@@ -3295,10 +3292,10 @@
         <v>3.0</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J58" s="5">
         <v>2.0</v>
@@ -3311,13 +3308,13 @@
         <v>4</v>
       </c>
       <c r="M58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N58" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O58" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="59">
@@ -3328,7 +3325,7 @@
         <v>16</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D59" s="4">
         <v>3312.0</v>
@@ -3362,10 +3359,10 @@
         <v>21</v>
       </c>
       <c r="N59" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O59" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O59" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="60">
@@ -3376,7 +3373,7 @@
         <v>16</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D60" s="4">
         <v>1087.0</v>
@@ -3394,7 +3391,7 @@
         <v>19</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J60" s="5">
         <v>3.0</v>
@@ -3407,13 +3404,13 @@
         <v>5</v>
       </c>
       <c r="M60" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N60" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O60" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="61">
@@ -3424,7 +3421,7 @@
         <v>16</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D61" s="4">
         <v>3332.0</v>
@@ -3439,7 +3436,7 @@
         <v>9.0</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I61" s="5" t="s">
         <v>20</v>
@@ -3458,10 +3455,10 @@
         <v>21</v>
       </c>
       <c r="N61" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O61" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O61" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="62">
@@ -3472,7 +3469,7 @@
         <v>16</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D62" s="4">
         <v>1490.0</v>
@@ -3506,10 +3503,10 @@
         <v>21</v>
       </c>
       <c r="N62" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O62" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O62" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="63">
@@ -3520,7 +3517,7 @@
         <v>16</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D63" s="4">
         <v>6053.0</v>
@@ -3538,7 +3535,7 @@
         <v>19</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J63" s="5">
         <v>2.0</v>
@@ -3551,13 +3548,13 @@
         <v>4</v>
       </c>
       <c r="M63" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N63" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O63" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="64">
@@ -3568,7 +3565,7 @@
         <v>16</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D64" s="4">
         <v>9845.0</v>
@@ -3602,10 +3599,10 @@
         <v>21</v>
       </c>
       <c r="N64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O64" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O64" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="65">
@@ -3616,7 +3613,7 @@
         <v>16</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D65" s="4">
         <v>8373.0</v>
@@ -3634,7 +3631,7 @@
         <v>19</v>
       </c>
       <c r="I65" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J65" s="5">
         <v>3.0</v>
@@ -3647,13 +3644,13 @@
         <v>5</v>
       </c>
       <c r="M65" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N65" s="5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="O65" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="66">
@@ -3664,7 +3661,7 @@
         <v>16</v>
       </c>
       <c r="C66" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D66" s="4">
         <v>3242.0</v>
@@ -3679,7 +3676,7 @@
         <v>12.0</v>
       </c>
       <c r="H66" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I66" s="5" t="s">
         <v>20</v>
@@ -3698,10 +3695,10 @@
         <v>21</v>
       </c>
       <c r="N66" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="O66" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="O66" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="67">

</xml_diff>